<commit_message>
Result export to excel
</commit_message>
<xml_diff>
--- a/DbScript/dbConfig/Enrollment/PersonNameActual/testdata.xlsx
+++ b/DbScript/dbConfig/Enrollment/PersonNameActual/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydutt\source\test\TestDataGen\DbScript\dbConfig\Enrollment\PersonNameActual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB94A51-8DEA-4EFD-AA40-C470D7FA7E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDF11C2-A00D-4067-BDC6-4D01B3B73ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,7 +384,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,7 +410,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -418,7 +418,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -426,7 +426,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -434,7 +434,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -442,7 +442,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -450,7 +450,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -458,7 +458,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -466,7 +466,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -474,7 +474,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -482,7 +482,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>

</xml_diff>